<commit_message>
Updated the input files in sixteen_tests to have strain_log2_expression instead of just strain and then ran the files and saved the outputs in sixteen_tests_output
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="25605" windowHeight="16005" tabRatio="644" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="25605" windowHeight="16005" tabRatio="644" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
     <sheet name="degradation_rates" sheetId="1" r:id="rId2"/>
-    <sheet name="wt" sheetId="17" r:id="rId3"/>
-    <sheet name="dcin5" sheetId="18" r:id="rId4"/>
+    <sheet name="wt_log2_expression" sheetId="17" r:id="rId3"/>
+    <sheet name="dcin5_log2_expression" sheetId="18" r:id="rId4"/>
     <sheet name="network" sheetId="5" r:id="rId5"/>
     <sheet name="network_weights" sheetId="11" r:id="rId6"/>
     <sheet name="optimization_parameters" sheetId="6" r:id="rId7"/>
@@ -1236,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
@@ -1784,7 +1784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
correct the input sheets for sixteen_tests and add the output sheets
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
@@ -15,7 +15,6 @@
     <sheet name="network_weights" sheetId="11" r:id="rId6"/>
     <sheet name="optimization_parameters" sheetId="6" r:id="rId7"/>
     <sheet name="threshold_b" sheetId="16" r:id="rId8"/>
-    <sheet name="ntoes" sheetId="19" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">network!$A$1:$V$22</definedName>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
   <si>
     <t>CIN5</t>
   </si>
@@ -115,9 +114,6 @@
   </si>
   <si>
     <t>dcin5</t>
-  </si>
-  <si>
-    <t>this is a test case in which the forward problem was solved to generate data.</t>
   </si>
   <si>
     <t>simtime</t>
@@ -970,7 +966,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1237,7 +1233,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1274,7 +1270,7 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="K1" s="10">
-        <v>1.2000000000000002</v>
+        <v>1.2</v>
       </c>
       <c r="L1" s="10">
         <v>1.6</v>
@@ -1785,7 +1781,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1871,7 +1867,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="9">
         <v>1</v>
@@ -1879,7 +1875,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="9">
         <v>1</v>
@@ -1915,7 +1911,7 @@
         <v>1.2</v>
       </c>
       <c r="E13">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1953,7 +1949,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2032,7 +2028,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2084,24 +2080,4 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the testing files according to the new beta version
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="25605" windowHeight="16005" tabRatio="644" activeTab="3"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="25605" windowHeight="16005" tabRatio="644" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -1232,7 +1232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -1780,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1814,7 +1814,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>1E-10</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1830,7 +1830,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="2">
-        <v>100000000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1838,7 +1838,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2">
-        <v>1E-10</v>
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1846,7 +1846,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2">
-        <v>100000000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1854,7 +1854,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="2">
-        <v>1E-10</v>
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Changed variable names on test_suite branch
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="25605" windowHeight="16005" tabRatio="644" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="25605" windowHeight="16005" tabRatio="644" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>CIN5</t>
   </si>
@@ -38,33 +38,12 @@
     <t>kk_max</t>
   </si>
   <si>
-    <t>SystematicName</t>
-  </si>
-  <si>
-    <t>StandardName</t>
-  </si>
-  <si>
-    <t>DegradationRate</t>
-  </si>
-  <si>
-    <t>YOR028C</t>
-  </si>
-  <si>
-    <t>YPR104C</t>
-  </si>
-  <si>
-    <t>rows genes affected/cols genes controlling</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
     <t>optimization_parameter</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>MaxIter</t>
   </si>
   <si>
@@ -77,21 +56,12 @@
     <t>TolX</t>
   </si>
   <si>
-    <t>YLR131C</t>
-  </si>
-  <si>
     <t>ACE2</t>
   </si>
   <si>
-    <t>production_rates</t>
-  </si>
-  <si>
     <t>AFT2</t>
   </si>
   <si>
-    <t>YPL202C</t>
-  </si>
-  <si>
     <t>Strain</t>
   </si>
   <si>
@@ -116,13 +86,31 @@
     <t>dcin5</t>
   </si>
   <si>
-    <t>simtime</t>
-  </si>
-  <si>
-    <t>estimateParams</t>
-  </si>
-  <si>
-    <t>makeGraphs</t>
+    <t>estimate_params</t>
+  </si>
+  <si>
+    <t>simulation_timepoints</t>
+  </si>
+  <si>
+    <t>make_graphs</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>production_rate</t>
+  </si>
+  <si>
+    <t>degradation_rate</t>
+  </si>
+  <si>
+    <t>regulators/controllers</t>
+  </si>
+  <si>
+    <t>threshold_b</t>
+  </si>
+  <si>
+    <t>expression_timepoints</t>
   </si>
 </sst>
 </file>
@@ -183,7 +171,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -200,6 +187,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,189 +593,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11" style="1"/>
+    <col min="1" max="1" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1"/>
       <c r="F1"/>
       <c r="G1"/>
-      <c r="H1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="B2">
         <v>0.5</v>
       </c>
-      <c r="H2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="H3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="H4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D4" s="5"/>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="H5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6" s="4"/>
-      <c r="H6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7" s="4"/>
-      <c r="H7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8" s="4"/>
-      <c r="H8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="4"/>
-      <c r="H9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10" s="4"/>
-      <c r="H10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11" s="4"/>
-      <c r="H11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12" s="4"/>
-      <c r="H12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="H13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14" s="4"/>
-      <c r="H14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15" s="4"/>
-      <c r="H15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16" s="4"/>
-      <c r="H16"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17" s="4"/>
-      <c r="H17"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18" s="4"/>
-      <c r="H18"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19" s="4"/>
-      <c r="E19" s="5"/>
-      <c r="H19"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20" s="4"/>
-      <c r="H20"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21"/>
-      <c r="C21"/>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
-      <c r="C22"/>
-      <c r="H22"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E24" s="5"/>
+      <c r="G22"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D24" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -799,159 +754,126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11" style="1"/>
+    <col min="1" max="1" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19"/>
-      <c r="C19"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="B20"/>
-      <c r="C20"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21"/>
-      <c r="C21"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
-      <c r="C22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -963,20 +885,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
+        <v>23</v>
+      </c>
+      <c r="B1" s="10">
+        <v>0.4</v>
       </c>
       <c r="C1" s="11">
         <v>0.4</v>
@@ -985,7 +907,7 @@
         <v>0.4</v>
       </c>
       <c r="E1" s="13">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="F1" s="14">
         <v>0.8</v>
@@ -994,16 +916,16 @@
         <v>0.8</v>
       </c>
       <c r="H1" s="16">
-        <v>0.8</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="I1" s="17">
         <v>1.2000000000000002</v>
       </c>
       <c r="J1" s="18">
-        <v>1.2000000000000002</v>
+        <v>1.2</v>
       </c>
       <c r="K1" s="19">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="L1" s="20">
         <v>1.6</v>
@@ -1011,17 +933,14 @@
       <c r="M1" s="21">
         <v>1.6</v>
       </c>
-      <c r="N1" s="22">
-        <v>1.6</v>
-      </c>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="10">
+        <v>-0.37633430629205178</v>
       </c>
       <c r="C2" s="11">
         <v>-0.37633430629205178</v>
@@ -1030,7 +949,7 @@
         <v>-0.37633430629205178</v>
       </c>
       <c r="E2" s="13">
-        <v>-0.37633430629205178</v>
+        <v>-0.70666646734338179</v>
       </c>
       <c r="F2" s="14">
         <v>-0.70666646734338179</v>
@@ -1039,7 +958,7 @@
         <v>-0.70666646734338179</v>
       </c>
       <c r="H2" s="16">
-        <v>-0.70666646734338179</v>
+        <v>-0.98723929967009216</v>
       </c>
       <c r="I2" s="17">
         <v>-0.98723929967009216</v>
@@ -1048,7 +967,7 @@
         <v>-0.98723929967009216</v>
       </c>
       <c r="K2" s="19">
-        <v>-0.98723929967009216</v>
+        <v>-1.2174432654761544</v>
       </c>
       <c r="L2" s="20">
         <v>-1.2174432654761544</v>
@@ -1056,16 +975,13 @@
       <c r="M2" s="21">
         <v>-1.2174432654761544</v>
       </c>
-      <c r="N2" s="22">
-        <v>-1.2174432654761544</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="10">
+        <v>-0.22771865423983556</v>
       </c>
       <c r="C3" s="11">
         <v>-0.22771865423983556</v>
@@ -1074,7 +990,7 @@
         <v>-0.22771865423983556</v>
       </c>
       <c r="E3" s="13">
-        <v>-0.22771865423983556</v>
+        <v>-0.40801774302656463</v>
       </c>
       <c r="F3" s="14">
         <v>-0.40801774302656463</v>
@@ -1083,7 +999,7 @@
         <v>-0.40801774302656463</v>
       </c>
       <c r="H3" s="16">
-        <v>-0.40801774302656463</v>
+        <v>-0.5464126532391167</v>
       </c>
       <c r="I3" s="17">
         <v>-0.5464126532391167</v>
@@ -1092,7 +1008,7 @@
         <v>-0.5464126532391167</v>
       </c>
       <c r="K3" s="19">
-        <v>-0.5464126532391167</v>
+        <v>-0.64984386018298912</v>
       </c>
       <c r="L3" s="20">
         <v>-0.64984386018298912</v>
@@ -1100,16 +1016,13 @@
       <c r="M3" s="21">
         <v>-0.64984386018298912</v>
       </c>
-      <c r="N3" s="22">
-        <v>-0.64984386018298912</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.26929382132237512</v>
       </c>
       <c r="C4" s="11">
         <v>0.26929382132237512</v>
@@ -1118,7 +1031,7 @@
         <v>0.26929382132237512</v>
       </c>
       <c r="E4" s="13">
-        <v>0.26929382132237512</v>
+        <v>0.41593537248224854</v>
       </c>
       <c r="F4" s="14">
         <v>0.41593537248224854</v>
@@ -1127,7 +1040,7 @@
         <v>0.41593537248224854</v>
       </c>
       <c r="H4" s="16">
-        <v>0.41593537248224854</v>
+        <v>0.49751163358969142</v>
       </c>
       <c r="I4" s="17">
         <v>0.49751163358969142</v>
@@ -1136,7 +1049,7 @@
         <v>0.49751163358969142</v>
       </c>
       <c r="K4" s="19">
-        <v>0.49751163358969142</v>
+        <v>0.54159993841241572</v>
       </c>
       <c r="L4" s="20">
         <v>0.54159993841241572</v>
@@ -1144,16 +1057,13 @@
       <c r="M4" s="21">
         <v>0.54159993841241572</v>
       </c>
-      <c r="N4" s="22">
-        <v>0.54159993841241572</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="10">
+        <v>-0.29093615522070321</v>
       </c>
       <c r="C5" s="11">
         <v>-0.29093615522070321</v>
@@ -1162,7 +1072,7 @@
         <v>-0.29093615522070321</v>
       </c>
       <c r="E5" s="13">
-        <v>-0.29093615522070321</v>
+        <v>-0.57977180156386388</v>
       </c>
       <c r="F5" s="14">
         <v>-0.57977180156386388</v>
@@ -1171,7 +1081,7 @@
         <v>-0.57977180156386388</v>
       </c>
       <c r="H5" s="16">
-        <v>-0.57977180156386388</v>
+        <v>-0.85583465653557034</v>
       </c>
       <c r="I5" s="17">
         <v>-0.85583465653557034</v>
@@ -1180,7 +1090,7 @@
         <v>-0.85583465653557034</v>
       </c>
       <c r="K5" s="19">
-        <v>-0.85583465653557034</v>
+        <v>-1.1097262320569594</v>
       </c>
       <c r="L5" s="20">
         <v>-1.1097262320569594</v>
@@ -1188,37 +1098,34 @@
       <c r="M5" s="21">
         <v>-1.1097262320569594</v>
       </c>
-      <c r="N5" s="22">
-        <v>-1.1097262320569594</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G6" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J10" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G12" s="2"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I14" s="2"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="I18" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="H18" s="2"/>
+      <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="F20" s="2"/>
-      <c r="M20" s="2"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="E20" s="2"/>
+      <c r="L20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1230,282 +1137,267 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="10">
+        <v>23</v>
+      </c>
+      <c r="B1" s="9">
         <v>0.4</v>
       </c>
-      <c r="D1" s="10">
+      <c r="C1" s="9">
         <v>0.4</v>
       </c>
-      <c r="E1" s="10">
+      <c r="D1" s="9">
         <v>0.4</v>
       </c>
-      <c r="F1" s="10">
+      <c r="E1" s="9">
         <v>0.8</v>
       </c>
-      <c r="G1" s="10">
+      <c r="F1" s="9">
         <v>0.8</v>
       </c>
-      <c r="H1" s="10">
+      <c r="G1" s="9">
         <v>0.8</v>
       </c>
-      <c r="I1" s="10">
+      <c r="H1" s="9">
         <v>1.2000000000000002</v>
       </c>
-      <c r="J1" s="10">
+      <c r="I1" s="9">
         <v>1.2000000000000002</v>
       </c>
-      <c r="K1" s="10">
+      <c r="J1" s="9">
         <v>1.2</v>
       </c>
-      <c r="L1" s="10">
+      <c r="K1" s="9">
         <v>1.6</v>
       </c>
-      <c r="M1" s="10">
+      <c r="L1" s="9">
         <v>1.6</v>
       </c>
-      <c r="N1" s="10">
+      <c r="M1" s="9">
         <v>1.6</v>
       </c>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="10">
+        <v>10</v>
+      </c>
+      <c r="B2" s="9">
         <v>-0.37633430629205178</v>
       </c>
-      <c r="D2" s="10">
+      <c r="C2" s="9">
         <v>-0.37633430629205178</v>
       </c>
-      <c r="E2" s="10">
+      <c r="D2" s="9">
         <v>-0.37633430629205178</v>
       </c>
-      <c r="F2" s="10">
+      <c r="E2" s="9">
         <v>-0.70666646734338179</v>
       </c>
-      <c r="G2" s="10">
+      <c r="F2" s="9">
         <v>-0.70666646734338179</v>
       </c>
-      <c r="H2" s="10">
+      <c r="G2" s="9">
         <v>-0.70666646734338179</v>
       </c>
-      <c r="I2" s="10">
+      <c r="H2" s="9">
         <v>-0.98723929967009216</v>
       </c>
-      <c r="J2" s="10">
+      <c r="I2" s="9">
         <v>-0.98723929967009216</v>
       </c>
-      <c r="K2" s="10">
+      <c r="J2" s="9">
         <v>-0.98723929967009216</v>
       </c>
-      <c r="L2" s="10">
+      <c r="K2" s="9">
         <v>-1.2174432654761544</v>
       </c>
-      <c r="M2" s="10">
+      <c r="L2" s="9">
         <v>-1.2174432654761544</v>
       </c>
-      <c r="N2" s="10">
+      <c r="M2" s="9">
         <v>-1.2174432654761544</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="10">
+        <v>11</v>
+      </c>
+      <c r="B3" s="9">
         <v>-0.22771865423983556</v>
       </c>
-      <c r="D3" s="10">
+      <c r="C3" s="9">
         <v>-0.22771865423983556</v>
       </c>
-      <c r="E3" s="10">
+      <c r="D3" s="9">
         <v>-0.22771865423983556</v>
       </c>
-      <c r="F3" s="10">
+      <c r="E3" s="9">
         <v>-0.40801774302656463</v>
       </c>
-      <c r="G3" s="10">
+      <c r="F3" s="9">
         <v>-0.40801774302656463</v>
       </c>
-      <c r="H3" s="10">
+      <c r="G3" s="9">
         <v>-0.40801774302656463</v>
       </c>
-      <c r="I3" s="10">
+      <c r="H3" s="9">
         <v>-0.5464126532391167</v>
       </c>
-      <c r="J3" s="10">
+      <c r="I3" s="9">
         <v>-0.5464126532391167</v>
       </c>
-      <c r="K3" s="10">
+      <c r="J3" s="9">
         <v>-0.5464126532391167</v>
       </c>
-      <c r="L3" s="10">
+      <c r="K3" s="9">
         <v>-0.64984386018298912</v>
       </c>
-      <c r="M3" s="10">
+      <c r="L3" s="9">
         <v>-0.64984386018298912</v>
       </c>
-      <c r="N3" s="10">
+      <c r="M3" s="9">
         <v>-0.64984386018298912</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="10">
-        <v>0</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10">
-        <v>0</v>
-      </c>
-      <c r="F4" s="10">
-        <v>0</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0</v>
-      </c>
-      <c r="I4" s="10">
-        <v>0</v>
-      </c>
-      <c r="J4" s="10">
-        <v>0</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0</v>
-      </c>
-      <c r="L4" s="10">
-        <v>0</v>
-      </c>
-      <c r="M4" s="10">
-        <v>0</v>
-      </c>
-      <c r="N4" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9">
         <v>-0.13932150464649004</v>
       </c>
-      <c r="D5" s="10">
+      <c r="C5" s="9">
         <v>-0.13932150464649004</v>
       </c>
-      <c r="E5" s="10">
+      <c r="D5" s="9">
         <v>-0.13932150464649004</v>
       </c>
-      <c r="F5" s="10">
+      <c r="E5" s="9">
         <v>-0.24985173044541253</v>
       </c>
-      <c r="G5" s="10">
+      <c r="F5" s="9">
         <v>-0.24985173044541253</v>
       </c>
-      <c r="H5" s="10">
+      <c r="G5" s="9">
         <v>-0.24985173044541253</v>
       </c>
-      <c r="I5" s="10">
+      <c r="H5" s="9">
         <v>-0.33614068837409528</v>
       </c>
-      <c r="J5" s="10">
+      <c r="I5" s="9">
         <v>-0.33614068837409528</v>
       </c>
-      <c r="K5" s="10">
+      <c r="J5" s="9">
         <v>-0.33614068837409528</v>
       </c>
-      <c r="L5" s="10">
+      <c r="K5" s="9">
         <v>-0.40259011361710589</v>
       </c>
-      <c r="M5" s="10">
+      <c r="L5" s="9">
         <v>-0.40259011361710589</v>
       </c>
-      <c r="N5" s="10">
+      <c r="M5" s="9">
         <v>-0.40259011361710589</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="L7" s="2"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F11" s="2"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C15" s="2"/>
-    </row>
-    <row r="18" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="G18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="I19" s="2"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="I20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="22" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="L22" s="2"/>
-      <c r="N22" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="18" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="H19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="H20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="22" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="K22" s="2"/>
+      <c r="M22" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1518,9 +1410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1545,14 +1435,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>9</v>
+      <c r="A1" s="22" t="s">
+        <v>26</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>0</v>
@@ -1563,7 +1453,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1580,7 +1470,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -1641,9 +1531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1667,14 +1555,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>9</v>
+      <c r="A1" s="22" t="s">
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1702,7 +1590,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1719,7 +1607,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -1781,7 +1669,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1791,22 +1679,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1827,7 +1715,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>1000000</v>
@@ -1835,7 +1723,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>1.0000000000000001E-5</v>
@@ -1843,7 +1731,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>1000000</v>
@@ -1851,7 +1739,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>1.0000000000000001E-5</v>
@@ -1859,49 +1747,49 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="9">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="9">
+        <v>20</v>
+      </c>
+      <c r="B9" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="9">
+        <v>22</v>
+      </c>
+      <c r="B10" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="9">
+        <v>15</v>
+      </c>
+      <c r="B11" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="9">
+        <v>16</v>
+      </c>
+      <c r="B12" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="9">
+        <v>28</v>
+      </c>
+      <c r="B13" s="8">
         <v>0.4</v>
       </c>
       <c r="C13">
@@ -1916,20 +1804,20 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="8">
+        <v>17</v>
+      </c>
+      <c r="B15" s="7">
         <v>3</v>
       </c>
       <c r="C15">
@@ -1938,9 +1826,9 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="8">
+        <v>13</v>
+      </c>
+      <c r="B16" s="7">
         <v>0</v>
       </c>
       <c r="C16">
@@ -1949,7 +1837,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2027,20 +1915,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
+      <c r="A1" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2048,7 +1939,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>

</xml_diff>

<commit_message>
Changed these files to have 'Model' instead of 'Sigmoid' optimization parameter
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
   <si>
     <t>CIN5</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Sheet</t>
   </si>
   <si>
-    <t>Sigmoid</t>
-  </si>
-  <si>
     <t>dcin5</t>
   </si>
   <si>
@@ -111,6 +108,12 @@
   </si>
   <si>
     <t>expression_timepoints</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>MM</t>
   </si>
 </sst>
 </file>
@@ -607,10 +610,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -769,10 +772,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -895,7 +898,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="10">
         <v>0.4</v>
@@ -1147,7 +1150,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="9">
         <v>0.4</v>
@@ -1436,7 +1439,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1556,7 +1559,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1669,7 +1672,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1747,15 +1750,15 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="8">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="8">
         <v>1</v>
@@ -1763,7 +1766,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="8">
         <v>1</v>
@@ -1787,7 +1790,7 @@
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="8">
         <v>0.4</v>
@@ -1810,7 +1813,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1837,7 +1840,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1923,10 +1926,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Changed sixteen sheets to include L-Curve parameter and changed model parameter to production_function.
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
   <si>
     <t>CIN5</t>
   </si>
@@ -107,20 +107,23 @@
     <t>expression_timepoints</t>
   </si>
   <si>
-    <t>Model</t>
-  </si>
-  <si>
     <t>MM</t>
   </si>
   <si>
     <t>targets/regulators</t>
+  </si>
+  <si>
+    <t>production_function</t>
+  </si>
+  <si>
+    <t>L_curve</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -145,6 +148,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -167,7 +175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -191,6 +199,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1439,7 +1448,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1559,7 +1568,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1669,10 +1678,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1750,23 +1759,23 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>19</v>
+      <c r="A9" s="23" t="s">
+        <v>30</v>
       </c>
       <c r="B9" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="8">
         <v>1</v>
@@ -1774,15 +1783,15 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>16</v>
       </c>
       <c r="B12" s="8">
         <v>0</v>
@@ -1790,126 +1799,134 @@
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B14" s="8">
         <v>0.4</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>0.8</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>1.2</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>1.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="7">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B16" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
         <v>0.1</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>0.2</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>0.30000000000000004</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>0.4</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>0.5</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>0.60000000000000009</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>0.70000000000000007</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>0.8</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>0.9</v>
       </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17">
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N17">
+      <c r="N18">
         <v>1.2000000000000002</v>
       </c>
-      <c r="O17">
+      <c r="O18">
         <v>1.3</v>
       </c>
-      <c r="P17">
+      <c r="P18">
         <v>1.4000000000000001</v>
       </c>
-      <c r="Q17">
+      <c r="Q18">
         <v>1.5</v>
       </c>
-      <c r="R17">
+      <c r="R18">
         <v>1.6</v>
       </c>
-      <c r="S17">
+      <c r="S18">
         <v>1.7000000000000002</v>
       </c>
-      <c r="T17">
+      <c r="T18">
         <v>1.8</v>
       </c>
-      <c r="U17">
+      <c r="U18">
         <v>1.9000000000000001</v>
       </c>
-      <c r="V17">
+      <c r="V18">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -1918,7 +1935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
removed deletion line on one file
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\r\GRNmap\test_files\sixteen_tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="3" activeTab="6"/>
   </bookViews>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
   <si>
     <t>CIN5</t>
   </si>
@@ -63,9 +68,6 @@
   </si>
   <si>
     <t>Strain</t>
-  </si>
-  <si>
-    <t>Deletion</t>
   </si>
   <si>
     <t>wt</t>
@@ -278,6 +280,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -619,10 +624,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -781,10 +786,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -907,7 +912,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="10">
         <v>0.4</v>
@@ -1159,7 +1164,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="9">
         <v>0.4</v>
@@ -1448,7 +1453,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1568,7 +1573,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1678,10 +1683,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1759,15 +1764,15 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="8">
         <v>0</v>
@@ -1775,7 +1780,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="8">
         <v>1</v>
@@ -1783,7 +1788,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
@@ -1791,7 +1796,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="8">
         <v>0</v>
@@ -1799,7 +1804,7 @@
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="8">
         <v>0</v>
@@ -1807,7 +1812,7 @@
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="8">
         <v>0.4</v>
@@ -1827,15 +1832,15 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="7">
         <v>3</v>
@@ -1846,80 +1851,69 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="7">
+        <v>19</v>
+      </c>
+      <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
         <v>0.1</v>
       </c>
-      <c r="D18">
+      <c r="D17">
         <v>0.2</v>
       </c>
-      <c r="E18">
+      <c r="E17">
         <v>0.30000000000000004</v>
       </c>
-      <c r="F18">
+      <c r="F17">
         <v>0.4</v>
       </c>
-      <c r="G18">
+      <c r="G17">
         <v>0.5</v>
       </c>
-      <c r="H18">
+      <c r="H17">
         <v>0.60000000000000009</v>
       </c>
-      <c r="I18">
+      <c r="I17">
         <v>0.70000000000000007</v>
       </c>
-      <c r="J18">
+      <c r="J17">
         <v>0.8</v>
       </c>
-      <c r="K18">
+      <c r="K17">
         <v>0.9</v>
       </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N18">
+      <c r="N17">
         <v>1.2000000000000002</v>
       </c>
-      <c r="O18">
+      <c r="O17">
         <v>1.3</v>
       </c>
-      <c r="P18">
+      <c r="P17">
         <v>1.4000000000000001</v>
       </c>
-      <c r="Q18">
+      <c r="Q17">
         <v>1.5</v>
       </c>
-      <c r="R18">
+      <c r="R17">
         <v>1.6</v>
       </c>
-      <c r="S18">
+      <c r="S17">
         <v>1.7000000000000002</v>
       </c>
-      <c r="T18">
+      <c r="T17">
         <v>1.8</v>
       </c>
-      <c r="U18">
+      <c r="U17">
         <v>1.9000000000000001</v>
       </c>
-      <c r="V18">
+      <c r="V17">
         <v>2</v>
       </c>
     </row>
@@ -1943,10 +1937,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>